<commit_message>
altered views to wait for database, finished up info pages except optimizer
</commit_message>
<xml_diff>
--- a/sector_MSE.xlsx
+++ b/sector_MSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fintech\Sample1\Dynamic-Stock-Recommendation-Machine_Learning-Published-Paper-IEEE-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyling/Desktop/BF3210 Issues in GFM/WWW/fintech_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F4145B-503C-4EBA-9E8B-5BE111103DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE340DC4-B7CA-2845-84A4-20A0E8F5FF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18732" yWindow="2016" windowWidth="17280" windowHeight="8964" xr2:uid="{49CEB546-F7A5-44FA-A9C9-A2800A9A1529}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" xr2:uid="{49CEB546-F7A5-44FA-A9C9-A2800A9A1529}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,54 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
+    <t>Consumer Discretionary</t>
+  </si>
+  <si>
+    <t>Consumer Staples</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Telecommunication Services</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,17 +105,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -382,185 +431,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E9D60F-8056-4E06-B4ED-E4DF669B6467}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B2" sqref="B2:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="1">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1">
-        <v>35</v>
-      </c>
-      <c r="G1" s="1">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1">
-        <v>45</v>
-      </c>
-      <c r="I1" s="1">
-        <v>50</v>
-      </c>
-      <c r="J1" s="1">
-        <v>55</v>
-      </c>
-      <c r="K1" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>20160901</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>42614</v>
+      </c>
+      <c r="B2" s="3">
         <v>3.1957149304599503E-2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>2.6822856514421199E-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>2.6534337275375099E-2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>1.04931209142147E-2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>1.7234613459241498E-2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>1.95174156430277E-2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>3.2957050074375098E-2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>2.0746304925583499E-2</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>1.8057341153116101E-2</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>1.1660783270304601E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>20161201</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B3" s="3">
         <v>3.1303839761281503E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>2.51424079953976E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>2.1687151785402699E-2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>1.1840382300255799E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>2.1639390284390998E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>2.9726620376135899E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>2.0677700936447E-2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>2.0135546211498899E-2</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>1.5885599882738501E-2</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>1.3829526163819999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>20170301</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>42795</v>
+      </c>
+      <c r="B4" s="3">
         <v>2.6084059952724399E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>2.2523912983547702E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>2.33046788125881E-2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>1.16045237384789E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>1.99561298199387E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>2.5212613096361601E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>2.24189301375495E-2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>1.9663001203128298E-2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>1.5889474634531098E-2</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>1.2764323572508699E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>20170601</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>42887</v>
+      </c>
+      <c r="B5" s="3">
         <v>2.7168443534278299E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>1.9383548981563001E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>2.2514150215916798E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>1.32931319611812E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>1.7571283060831298E-2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>2.10088225724279E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>2.02811641940214E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>5.2212835115111801E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>1.15207225631351E-2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>1.4801152413243399E-2</v>
       </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>